<commit_message>
update confusion matrix after deleteing first 10 rows of  data
</commit_message>
<xml_diff>
--- a/Documents/Note/ConfusionMatrix.xlsx
+++ b/Documents/Note/ConfusionMatrix.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester3\ML-AIS\ML-AIS-Sensor-Project-2021\Documents\Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A398FA4-5937-4577-9FF2-08C78C00CFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D52CA9-349D-41F8-AE37-7AD5F4755773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="-120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
+    <sheet name="Confusion Matrix" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Confusion Matrix</t>
   </si>
@@ -40,6 +49,12 @@
   </si>
   <si>
     <t>Total Measurements with Headers</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Deleting first 10 rows</t>
   </si>
 </sst>
 </file>
@@ -71,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -94,14 +109,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -123,14 +149,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -161,12 +187,73 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2476500" y="1905000"/>
+          <a:off x="0" y="2476500"/>
           <a:ext cx="5334000" cy="4000500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D474E36-F0F7-4114-8EDD-42628906EC7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7172325" y="1905000"/>
+          <a:ext cx="5324475" cy="3990975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -471,55 +558,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5" s="1">
         <v>843</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <f>J6+J7</f>
+        <v>843</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>719</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
         <v>124</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8" s="1">
         <v>41571</v>
       </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="I8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1">
+        <v>34383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+      <c r="G33" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -529,18 +768,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -690,6 +929,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCE22B4B-37F6-45BD-A1C9-1DD2BC55345B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59875E47-066E-4085-96D0-3464E0F44A34}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -701,14 +948,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCE22B4B-37F6-45BD-A1C9-1DD2BC55345B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>